<commit_message>
Vacaciones pendientes - consulta: revisión general y leves correcciones.
</commit_message>
<xml_diff>
--- a/Temp/VacacionesDiasPendientes_manuel.xlsx
+++ b/Temp/VacacionesDiasPendientes_manuel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <x:si>
     <x:t>Años de vacaciones</x:t>
   </x:si>
@@ -79,7 +79,49 @@
     <x:t>Este año</x:t>
   </x:si>
   <x:si>
-    <x:t>MERCYE.SOSAR.</x:t>
+    <x:t>MARIAEUGENIA</x:t>
+  </x:si>
+  <x:si>
+    <x:t>28-11-2001</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-11-2002</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-09-2004</x:t>
+  </x:si>
+  <x:si>
+    <x:t>17-11-2006</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20-11-2007</x:t>
+  </x:si>
+  <x:si>
+    <x:t>28-03-2008</x:t>
+  </x:si>
+  <x:si>
+    <x:t>22-06-2009</x:t>
+  </x:si>
+  <x:si>
+    <x:t>14-01-2011</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30-09-2011</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16-11-2012</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13-11-2014</x:t>
+  </x:si>
+  <x:si>
+    <x:t>23-11-2015</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15-02-2016</x:t>
+  </x:si>
+  <x:si>
+    <x:t>31-07-2019</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -635,17 +677,17 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:R17"/>
+  <x:dimension ref="A1:R23"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
     <x:col min="1" max="1" width="9.140625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="16.980625" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="16.840625000000003" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="4.130625" style="10" customWidth="1"/>
     <x:col min="4" max="4" width="10.700625" style="10" customWidth="1"/>
-    <x:col min="5" max="5" width="11.700625" style="10" customWidth="1"/>
+    <x:col min="5" max="5" width="12.410625" style="10" customWidth="1"/>
     <x:col min="6" max="6" width="7.840625" style="10" customWidth="1"/>
     <x:col min="7" max="7" width="6.550625" style="10" customWidth="1"/>
     <x:col min="8" max="8" width="8.550625" style="10" customWidth="1"/>
@@ -769,10 +811,10 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="D5" s="11">
-        <x:v>38169</x:v>
+        <x:v>36923</x:v>
       </x:c>
       <x:c r="E5" s="11">
-        <x:v>38533</x:v>
+        <x:v>37257</x:v>
       </x:c>
       <x:c r="F5" s="10" t="n">
         <x:v>15</x:v>
@@ -790,28 +832,28 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="K5" s="11">
-        <x:v>38208</x:v>
-      </x:c>
-      <x:c r="L5" s="11">
-        <x:v>38434</x:v>
+        <x:v>37049</x:v>
+      </x:c>
+      <x:c r="L5" s="10" t="s">
+        <x:v>22</x:v>
       </x:c>
       <x:c r="M5" s="10" t="n">
-        <x:v>31</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="N5" s="10" t="n">
-        <x:v>7</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="O5" s="10" t="n">
-        <x:v>24</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="P5" s="10" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="Q5" s="10" t="n">
-        <x:v>-9</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="R5" s="10" t="n">
-        <x:v>-9</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:18">
@@ -822,10 +864,10 @@
         <x:v>2</x:v>
       </x:c>
       <x:c r="D6" s="11">
-        <x:v>38534</x:v>
+        <x:v>37288</x:v>
       </x:c>
       <x:c r="E6" s="11">
-        <x:v>38898</x:v>
+        <x:v>37622</x:v>
       </x:c>
       <x:c r="F6" s="10" t="n">
         <x:v>16</x:v>
@@ -840,31 +882,31 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="J6" s="10" t="n">
-        <x:v>4</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="K6" s="11">
-        <x:v>38580</x:v>
-      </x:c>
-      <x:c r="L6" s="11">
-        <x:v>38849</x:v>
+        <x:v>37288</x:v>
+      </x:c>
+      <x:c r="L6" s="10" t="s">
+        <x:v>23</x:v>
       </x:c>
       <x:c r="M6" s="10" t="n">
-        <x:v>18</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="N6" s="10" t="n">
-        <x:v>4</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="O6" s="10" t="n">
-        <x:v>14</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="P6" s="10" t="n">
-        <x:v>-9</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="Q6" s="10" t="n">
-        <x:v>2</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="R6" s="10" t="n">
-        <x:v>-7</x:v>
+        <x:v>16</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:18">
@@ -875,10 +917,10 @@
         <x:v>3</x:v>
       </x:c>
       <x:c r="D7" s="11">
-        <x:v>38899</x:v>
+        <x:v>37653</x:v>
       </x:c>
       <x:c r="E7" s="11">
-        <x:v>39263</x:v>
+        <x:v>37987</x:v>
       </x:c>
       <x:c r="F7" s="10" t="n">
         <x:v>17</x:v>
@@ -893,31 +935,31 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="J7" s="10" t="n">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="K7" s="11">
-        <x:v>38929</x:v>
+        <x:v>37653</x:v>
       </x:c>
       <x:c r="L7" s="11">
-        <x:v>39202</x:v>
+        <x:v>37664</x:v>
       </x:c>
       <x:c r="M7" s="10" t="n">
-        <x:v>38</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="N7" s="10" t="n">
-        <x:v>9</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="O7" s="10" t="n">
-        <x:v>29</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="P7" s="10" t="n">
-        <x:v>-7</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="Q7" s="10" t="n">
-        <x:v>-12</x:v>
+        <x:v>-6</x:v>
       </x:c>
       <x:c r="R7" s="10" t="n">
-        <x:v>-19</x:v>
+        <x:v>10</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:18">
@@ -928,10 +970,10 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="D8" s="11">
-        <x:v>39264</x:v>
+        <x:v>38018</x:v>
       </x:c>
       <x:c r="E8" s="11">
-        <x:v>39629</x:v>
+        <x:v>38353</x:v>
       </x:c>
       <x:c r="F8" s="10" t="n">
         <x:v>18</x:v>
@@ -946,31 +988,31 @@
         <x:v>18</x:v>
       </x:c>
       <x:c r="J8" s="10" t="n">
-        <x:v>3</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="K8" s="11">
-        <x:v>39269</x:v>
-      </x:c>
-      <x:c r="L8" s="11">
-        <x:v>39624</x:v>
+        <x:v>38200</x:v>
+      </x:c>
+      <x:c r="L8" s="10" t="s">
+        <x:v>24</x:v>
       </x:c>
       <x:c r="M8" s="10" t="n">
-        <x:v>16</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="N8" s="10" t="n">
-        <x:v>3</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="O8" s="10" t="n">
-        <x:v>13</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="P8" s="10" t="n">
-        <x:v>-19</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="Q8" s="10" t="n">
-        <x:v>5</x:v>
+        <x:v>-1</x:v>
       </x:c>
       <x:c r="R8" s="10" t="n">
-        <x:v>-14</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:18">
@@ -981,10 +1023,10 @@
         <x:v>5</x:v>
       </x:c>
       <x:c r="D9" s="11">
-        <x:v>39630</x:v>
+        <x:v>38384</x:v>
       </x:c>
       <x:c r="E9" s="11">
-        <x:v>39994</x:v>
+        <x:v>38718</x:v>
       </x:c>
       <x:c r="F9" s="10" t="n">
         <x:v>19</x:v>
@@ -999,31 +1041,31 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="J9" s="10" t="n">
-        <x:v>4</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="K9" s="11">
-        <x:v>39780</x:v>
+        <x:v>38657</x:v>
       </x:c>
       <x:c r="L9" s="11">
-        <x:v>39990</x:v>
+        <x:v>38667</x:v>
       </x:c>
       <x:c r="M9" s="10" t="n">
-        <x:v>6</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="N9" s="10" t="n">
-        <x:v>0</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="O9" s="10" t="n">
-        <x:v>6</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="P9" s="10" t="n">
-        <x:v>-14</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="Q9" s="10" t="n">
-        <x:v>13</x:v>
+        <x:v>-4</x:v>
       </x:c>
       <x:c r="R9" s="10" t="n">
-        <x:v>-1</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:18">
@@ -1034,10 +1076,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="D10" s="11">
-        <x:v>39995</x:v>
+        <x:v>38749</x:v>
       </x:c>
       <x:c r="E10" s="11">
-        <x:v>40359</x:v>
+        <x:v>39083</x:v>
       </x:c>
       <x:c r="F10" s="10" t="n">
         <x:v>20</x:v>
@@ -1052,31 +1094,31 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="J10" s="10" t="n">
-        <x:v>1</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="K10" s="11">
-        <x:v>40028</x:v>
-      </x:c>
-      <x:c r="L10" s="11">
-        <x:v>40046</x:v>
+        <x:v>38991</x:v>
+      </x:c>
+      <x:c r="L10" s="10" t="s">
+        <x:v>25</x:v>
       </x:c>
       <x:c r="M10" s="10" t="n">
-        <x:v>19</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="N10" s="10" t="n">
-        <x:v>4</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="O10" s="10" t="n">
-        <x:v>15</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="P10" s="10" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="Q10" s="10" t="n">
+        <x:v>-6</x:v>
+      </x:c>
+      <x:c r="R10" s="10" t="n">
         <x:v>-1</x:v>
-      </x:c>
-      <x:c r="Q10" s="10" t="n">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="R10" s="10" t="n">
-        <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:18">
@@ -1087,10 +1129,10 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="D11" s="11">
-        <x:v>40360</x:v>
+        <x:v>39114</x:v>
       </x:c>
       <x:c r="E11" s="11">
-        <x:v>40724</x:v>
+        <x:v>39448</x:v>
       </x:c>
       <x:c r="F11" s="10" t="n">
         <x:v>21</x:v>
@@ -1105,31 +1147,31 @@
         <x:v>21</x:v>
       </x:c>
       <x:c r="J11" s="10" t="n">
-        <x:v>2</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="K11" s="11">
-        <x:v>40361</x:v>
-      </x:c>
-      <x:c r="L11" s="11">
-        <x:v>40452</x:v>
+        <x:v>39295</x:v>
+      </x:c>
+      <x:c r="L11" s="10" t="s">
+        <x:v>26</x:v>
       </x:c>
       <x:c r="M11" s="10" t="n">
-        <x:v>30</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="N11" s="10" t="n">
         <x:v>9</x:v>
       </x:c>
       <x:c r="O11" s="10" t="n">
-        <x:v>21</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="P11" s="10" t="n">
-        <x:v>4</x:v>
+        <x:v>-1</x:v>
       </x:c>
       <x:c r="Q11" s="10" t="n">
-        <x:v>0</x:v>
+        <x:v>-5</x:v>
       </x:c>
       <x:c r="R11" s="10" t="n">
-        <x:v>4</x:v>
+        <x:v>-6</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:18">
@@ -1140,10 +1182,10 @@
         <x:v>8</x:v>
       </x:c>
       <x:c r="D12" s="11">
-        <x:v>40725</x:v>
+        <x:v>39479</x:v>
       </x:c>
       <x:c r="E12" s="11">
-        <x:v>41090</x:v>
+        <x:v>39814</x:v>
       </x:c>
       <x:c r="F12" s="10" t="n">
         <x:v>22</x:v>
@@ -1158,31 +1200,31 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="J12" s="10" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="K12" s="11">
-        <x:v>40742</x:v>
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="K12" s="10" t="s">
+        <x:v>27</x:v>
       </x:c>
       <x:c r="L12" s="11">
-        <x:v>41044</x:v>
+        <x:v>39732</x:v>
       </x:c>
       <x:c r="M12" s="10" t="n">
-        <x:v>28</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="N12" s="10" t="n">
-        <x:v>6</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="O12" s="10" t="n">
         <x:v>22</x:v>
       </x:c>
       <x:c r="P12" s="10" t="n">
-        <x:v>4</x:v>
+        <x:v>-6</x:v>
       </x:c>
       <x:c r="Q12" s="10" t="n">
         <x:v>0</x:v>
       </x:c>
       <x:c r="R12" s="10" t="n">
-        <x:v>4</x:v>
+        <x:v>-6</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:18">
@@ -1193,10 +1235,10 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="D13" s="11">
-        <x:v>41091</x:v>
+        <x:v>39845</x:v>
       </x:c>
       <x:c r="E13" s="11">
-        <x:v>41455</x:v>
+        <x:v>40179</x:v>
       </x:c>
       <x:c r="F13" s="10" t="n">
         <x:v>23</x:v>
@@ -1211,31 +1253,31 @@
         <x:v>23</x:v>
       </x:c>
       <x:c r="J13" s="10" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="K13" s="11">
+        <x:v>40092</x:v>
+      </x:c>
+      <x:c r="L13" s="10" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="M13" s="10" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="N13" s="10" t="n">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="K13" s="11">
-        <x:v>41096</x:v>
-      </x:c>
-      <x:c r="L13" s="11">
-        <x:v>41351</x:v>
-      </x:c>
-      <x:c r="M13" s="10" t="n">
-        <x:v>42</x:v>
-      </x:c>
-      <x:c r="N13" s="10" t="n">
-        <x:v>12</x:v>
-      </x:c>
       <x:c r="O13" s="10" t="n">
-        <x:v>30</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="P13" s="10" t="n">
-        <x:v>4</x:v>
+        <x:v>-6</x:v>
       </x:c>
       <x:c r="Q13" s="10" t="n">
-        <x:v>-7</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="R13" s="10" t="n">
-        <x:v>-3</x:v>
+        <x:v>9</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:18">
@@ -1246,10 +1288,10 @@
         <x:v>10</x:v>
       </x:c>
       <x:c r="D14" s="11">
-        <x:v>41456</x:v>
+        <x:v>40210</x:v>
       </x:c>
       <x:c r="E14" s="11">
-        <x:v>41820</x:v>
+        <x:v>40544</x:v>
       </x:c>
       <x:c r="F14" s="10" t="n">
         <x:v>24</x:v>
@@ -1267,28 +1309,28 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="K14" s="11">
-        <x:v>41495</x:v>
+        <x:v>40483</x:v>
       </x:c>
       <x:c r="L14" s="11">
-        <x:v>41663</x:v>
+        <x:v>40519</x:v>
       </x:c>
       <x:c r="M14" s="10" t="n">
-        <x:v>39</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="N14" s="10" t="n">
-        <x:v>15</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="O14" s="10" t="n">
-        <x:v>24</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="P14" s="10" t="n">
-        <x:v>-3</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="Q14" s="10" t="n">
-        <x:v>0</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="R14" s="10" t="n">
-        <x:v>-3</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:18">
@@ -1299,10 +1341,10 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="D15" s="11">
-        <x:v>41821</x:v>
+        <x:v>40575</x:v>
       </x:c>
       <x:c r="E15" s="11">
-        <x:v>42185</x:v>
+        <x:v>40909</x:v>
       </x:c>
       <x:c r="F15" s="10" t="n">
         <x:v>25</x:v>
@@ -1317,31 +1359,31 @@
         <x:v>25</x:v>
       </x:c>
       <x:c r="J15" s="10" t="n">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="K15" s="11">
-        <x:v>41845</x:v>
-      </x:c>
-      <x:c r="L15" s="11">
-        <x:v>42083</x:v>
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="K15" s="10" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="L15" s="10" t="s">
+        <x:v>30</x:v>
       </x:c>
       <x:c r="M15" s="10" t="n">
-        <x:v>29</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="N15" s="10" t="n">
-        <x:v>6</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="O15" s="10" t="n">
-        <x:v>23</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="P15" s="10" t="n">
-        <x:v>-3</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="Q15" s="10" t="n">
-        <x:v>2</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="R15" s="10" t="n">
-        <x:v>-1</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="16" spans="1:18">
@@ -1352,10 +1394,10 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="D16" s="11">
-        <x:v>42186</x:v>
+        <x:v>40940</x:v>
       </x:c>
       <x:c r="E16" s="11">
-        <x:v>42551</x:v>
+        <x:v>41275</x:v>
       </x:c>
       <x:c r="F16" s="10" t="n">
         <x:v>26</x:v>
@@ -1370,31 +1412,31 @@
         <x:v>26</x:v>
       </x:c>
       <x:c r="J16" s="10" t="n">
-        <x:v>3</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="K16" s="11">
-        <x:v>42321</x:v>
-      </x:c>
-      <x:c r="L16" s="11">
-        <x:v>42432</x:v>
+        <x:v>40940</x:v>
+      </x:c>
+      <x:c r="L16" s="10" t="s">
+        <x:v>31</x:v>
       </x:c>
       <x:c r="M16" s="10" t="n">
-        <x:v>28</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="N16" s="10" t="n">
-        <x:v>7</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="O16" s="10" t="n">
-        <x:v>21</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="P16" s="10" t="n">
-        <x:v>-1</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="Q16" s="10" t="n">
-        <x:v>5</x:v>
+        <x:v>-6</x:v>
       </x:c>
       <x:c r="R16" s="10" t="n">
-        <x:v>4</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="17" spans="1:18">
@@ -1405,49 +1447,355 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="D17" s="11">
-        <x:v>42552</x:v>
+        <x:v>41306</x:v>
       </x:c>
       <x:c r="E17" s="11">
-        <x:v>42763</x:v>
+        <x:v>41640</x:v>
       </x:c>
       <x:c r="F17" s="10" t="n">
         <x:v>27</x:v>
       </x:c>
       <x:c r="G17" s="10" t="n">
-        <x:v>211</x:v>
+        <x:v>360</x:v>
       </x:c>
       <x:c r="H17" s="10" t="n">
-        <x:v>0.5861</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="I17" s="10" t="n">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="J17" s="10" t="n">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="K17" s="11">
+        <x:v>41306</x:v>
+      </x:c>
+      <x:c r="L17" s="11">
+        <x:v>41588</x:v>
+      </x:c>
+      <x:c r="M17" s="10" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="N17" s="10" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="O17" s="10" t="n">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="P17" s="10" t="n">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="Q17" s="10" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="R17" s="10" t="n">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:18">
+      <x:c r="B18" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C18" s="10" t="n">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="D18" s="11">
+        <x:v>41671</x:v>
+      </x:c>
+      <x:c r="E18" s="11">
+        <x:v>42005</x:v>
+      </x:c>
+      <x:c r="F18" s="10" t="n">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="G18" s="10" t="n">
+        <x:v>360</x:v>
+      </x:c>
+      <x:c r="H18" s="10" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I18" s="10" t="n">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="J18" s="10" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="K18" s="11">
+        <x:v>41671</x:v>
+      </x:c>
+      <x:c r="L18" s="10" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="M18" s="10" t="n">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="N18" s="10" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="O18" s="10" t="n">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="P18" s="10" t="n">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="Q18" s="10" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="R18" s="10" t="n">
+        <x:v>12</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:18">
+      <x:c r="B19" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C19" s="10" t="n">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="D19" s="11">
+        <x:v>42036</x:v>
+      </x:c>
+      <x:c r="E19" s="11">
+        <x:v>42370</x:v>
+      </x:c>
+      <x:c r="F19" s="10" t="n">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="G19" s="10" t="n">
+        <x:v>360</x:v>
+      </x:c>
+      <x:c r="H19" s="10" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I19" s="10" t="n">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="J19" s="10" t="n">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="K19" s="11">
+        <x:v>42036</x:v>
+      </x:c>
+      <x:c r="L19" s="10" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="M19" s="10" t="n">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="N19" s="10" t="n">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="O19" s="10" t="n">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="P19" s="10" t="n">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="Q19" s="10" t="n">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="R19" s="10" t="n">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:18">
+      <x:c r="B20" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C20" s="10" t="n">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="J17" s="10" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="K17" s="11">
-        <x:v>42590</x:v>
-      </x:c>
-      <x:c r="L17" s="11">
-        <x:v>42642</x:v>
-      </x:c>
-      <x:c r="M17" s="10" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="N17" s="10" t="n">
+      <x:c r="D20" s="11">
+        <x:v>42401</x:v>
+      </x:c>
+      <x:c r="E20" s="11">
+        <x:v>42736</x:v>
+      </x:c>
+      <x:c r="F20" s="10" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="G20" s="10" t="n">
+        <x:v>360</x:v>
+      </x:c>
+      <x:c r="H20" s="10" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I20" s="10" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J20" s="10" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="K20" s="10" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="L20" s="11">
+        <x:v>42624</x:v>
+      </x:c>
+      <x:c r="M20" s="10" t="n">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="N20" s="10" t="n">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="O20" s="10" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="P20" s="10" t="n">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="Q20" s="10" t="n">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="R20" s="10" t="n">
+        <x:v>33</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="21" spans="1:18">
+      <x:c r="B21" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C21" s="10" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D21" s="11">
+        <x:v>42767</x:v>
+      </x:c>
+      <x:c r="E21" s="11">
+        <x:v>43101</x:v>
+      </x:c>
+      <x:c r="F21" s="10" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="G21" s="10" t="n">
+        <x:v>360</x:v>
+      </x:c>
+      <x:c r="H21" s="10" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I21" s="10" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J21" s="10" t="n">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="O17" s="10" t="n">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="P17" s="10" t="n">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="Q17" s="10" t="n">
-        <x:v>14</x:v>
-      </x:c>
-      <x:c r="R17" s="10" t="n">
+      <x:c r="K21" s="10" t="s"/>
+      <x:c r="L21" s="10" t="s"/>
+      <x:c r="M21" s="10" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="N21" s="10" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="O21" s="10" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="P21" s="10" t="n">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="Q21" s="10" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="R21" s="10" t="n">
+        <x:v>63</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:18">
+      <x:c r="B22" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C22" s="10" t="n">
         <x:v>18</x:v>
+      </x:c>
+      <x:c r="D22" s="11">
+        <x:v>43132</x:v>
+      </x:c>
+      <x:c r="E22" s="11">
+        <x:v>43466</x:v>
+      </x:c>
+      <x:c r="F22" s="10" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="G22" s="10" t="n">
+        <x:v>360</x:v>
+      </x:c>
+      <x:c r="H22" s="10" t="n">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="I22" s="10" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="J22" s="10" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K22" s="10" t="s"/>
+      <x:c r="L22" s="10" t="s"/>
+      <x:c r="M22" s="10" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="N22" s="10" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="O22" s="10" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="P22" s="10" t="n">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="Q22" s="10" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="R22" s="10" t="n">
+        <x:v>93</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:18">
+      <x:c r="B23" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="C23" s="10" t="n">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D23" s="11">
+        <x:v>43497</x:v>
+      </x:c>
+      <x:c r="E23" s="10" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="F23" s="10" t="n">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="G23" s="10" t="n">
+        <x:v>210</x:v>
+      </x:c>
+      <x:c r="H23" s="10" t="n">
+        <x:v>0.5833</x:v>
+      </x:c>
+      <x:c r="I23" s="10" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="J23" s="10" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="K23" s="10" t="s"/>
+      <x:c r="L23" s="10" t="s"/>
+      <x:c r="M23" s="10" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="N23" s="10" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="O23" s="10" t="n">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="P23" s="10" t="n">
+        <x:v>93</x:v>
+      </x:c>
+      <x:c r="Q23" s="10" t="n">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="R23" s="10" t="n">
+        <x:v>110</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>